<commit_message>
Fixed bug for Trastuzumab-Emtancina molecule in part_2.py
</commit_message>
<xml_diff>
--- a/Control/New_Market_Basket.xlsx
+++ b/Control/New_Market_Basket.xlsx
@@ -5,25 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Final_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hriti\OneDrive\Desktop\Roche_Projects\Chile_Data_Acquisition\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FBAB08-8576-401A-921F-7C6FA3FF3E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D9FAC6-1E0C-48D2-B973-EE9F92FE88C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Market Basket" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final Market Basket'!$A$1:$G$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final Market Basket'!$A$1:$G$153</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="219">
   <si>
     <t>Market or TA</t>
   </si>
@@ -674,13 +674,19 @@
   </si>
   <si>
     <t>INTERFERON BETA 1A PEGILADO</t>
+  </si>
+  <si>
+    <t>TRASTUZUMAB EMTANZSINA</t>
+  </si>
+  <si>
+    <t>Trastuzumab etamsine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -692,31 +698,43 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -808,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -828,6 +846,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,10 +1065,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3233,60 +3252,56 @@
       <c r="A96" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D98" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E97" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A98" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>10</v>
@@ -3300,15 +3315,17 @@
     </row>
     <row r="99" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D99" s="4"/>
+        <v>138</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E99" s="4" t="s">
         <v>10</v>
       </c>
@@ -3316,7 +3333,7 @@
         <v>10</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -3324,13 +3341,13 @@
         <v>140</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>10</v>
@@ -3347,14 +3364,12 @@
         <v>140</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
         <v>10</v>
       </c>
@@ -3362,21 +3377,21 @@
         <v>10</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>10</v>
@@ -3390,16 +3405,16 @@
     </row>
     <row r="103" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>10</v>
@@ -3413,16 +3428,16 @@
     </row>
     <row r="104" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>10</v>
@@ -3436,16 +3451,16 @@
     </row>
     <row r="105" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>10</v>
@@ -3468,7 +3483,7 @@
         <v>152</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>10</v>
@@ -3482,16 +3497,16 @@
     </row>
     <row r="107" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>10</v>
@@ -3505,15 +3520,17 @@
     </row>
     <row r="108" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D108" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="E108" s="4" t="s">
         <v>10</v>
       </c>
@@ -3521,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -3529,13 +3546,13 @@
         <v>156</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>10</v>
@@ -3552,10 +3569,10 @@
         <v>156</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4" t="s">
@@ -3569,17 +3586,17 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>164</v>
+      <c r="A111" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>10</v>
@@ -3592,18 +3609,16 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A112" s="11" t="s">
-        <v>163</v>
+      <c r="A112" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>167</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>10</v>
       </c>
@@ -3611,21 +3626,21 @@
         <v>10</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B113" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>168</v>
+      <c r="B113" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>10</v>
@@ -3642,13 +3657,13 @@
         <v>163</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>10</v>
@@ -3665,13 +3680,13 @@
         <v>163</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>10</v>
@@ -3688,13 +3703,13 @@
         <v>163</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>10</v>
@@ -3711,13 +3726,13 @@
         <v>163</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>10</v>
@@ -3740,7 +3755,7 @@
         <v>173</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>10</v>
@@ -3763,7 +3778,7 @@
         <v>173</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>10</v>
@@ -3786,62 +3801,62 @@
         <v>173</v>
       </c>
       <c r="D120" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A122" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E120" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F120" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E121" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G121" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="E122" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -3849,22 +3864,22 @@
         <v>179</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -3878,7 +3893,7 @@
         <v>182</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>40</v>
@@ -3901,7 +3916,7 @@
         <v>182</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>40</v>
@@ -3924,7 +3939,7 @@
         <v>182</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>40</v>
@@ -3947,7 +3962,7 @@
         <v>182</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>40</v>
@@ -3970,7 +3985,7 @@
         <v>182</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>40</v>
@@ -3987,22 +4002,22 @@
         <v>179</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -4010,17 +4025,19 @@
         <v>179</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D130" s="4"/>
+        <v>182</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="E130" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>40</v>
@@ -4031,12 +4048,14 @@
         <v>179</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D131" s="4"/>
+      <c r="D131" s="4" t="s">
+        <v>191</v>
+      </c>
       <c r="E131" s="4" t="s">
         <v>10</v>
       </c>
@@ -4044,7 +4063,7 @@
         <v>10</v>
       </c>
       <c r="G131" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -4052,7 +4071,7 @@
         <v>179</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>190</v>
@@ -4073,7 +4092,7 @@
         <v>179</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>190</v>
@@ -4093,8 +4112,8 @@
       <c r="A134" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B134" s="6" t="s">
-        <v>196</v>
+      <c r="B134" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>190</v>
@@ -4115,14 +4134,12 @@
         <v>179</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>198</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
         <v>10</v>
       </c>
@@ -4130,22 +4147,20 @@
         <v>10</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>197</v>
+      <c r="B136" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>199</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D136" s="4"/>
       <c r="E136" s="4" t="s">
         <v>10</v>
       </c>
@@ -4153,7 +4168,7 @@
         <v>10</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -4167,7 +4182,7 @@
         <v>197</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>10</v>
@@ -4190,7 +4205,7 @@
         <v>197</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>10</v>
@@ -4213,7 +4228,7 @@
         <v>197</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>10</v>
@@ -4236,7 +4251,7 @@
         <v>197</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>10</v>
@@ -4253,12 +4268,14 @@
         <v>179</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D141" s="4"/>
+      <c r="D141" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="E141" s="4" t="s">
         <v>10</v>
       </c>
@@ -4266,7 +4283,7 @@
         <v>10</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -4274,12 +4291,14 @@
         <v>179</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D142" s="4"/>
+      <c r="D142" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="E142" s="4" t="s">
         <v>10</v>
       </c>
@@ -4287,7 +4306,7 @@
         <v>10</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
@@ -4295,7 +4314,7 @@
         <v>179</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>197</v>
@@ -4316,7 +4335,7 @@
         <v>179</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>197</v>
@@ -4337,7 +4356,7 @@
         <v>179</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>197</v>
@@ -4357,13 +4376,13 @@
       <c r="A146" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B146" s="6" t="s">
-        <v>209</v>
+      <c r="B146" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D146" s="6"/>
+      <c r="D146" s="4"/>
       <c r="E146" s="4" t="s">
         <v>10</v>
       </c>
@@ -4378,13 +4397,13 @@
       <c r="A147" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B147" s="6" t="s">
-        <v>210</v>
+      <c r="B147" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D147" s="6"/>
+      <c r="D147" s="4"/>
       <c r="E147" s="4" t="s">
         <v>10</v>
       </c>
@@ -4400,7 +4419,7 @@
         <v>179</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>197</v>
@@ -4417,74 +4436,116 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A149" s="14" t="s">
+      <c r="A149" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D149" s="6"/>
+      <c r="E149" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G149" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A150" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D150" s="6"/>
+      <c r="E150" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G150" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A151" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B151" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C151" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D151" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E149" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F149" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G149" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="10" t="s">
+      <c r="E151" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G151" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B150" s="8" t="s">
+      <c r="B152" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C150" s="8" t="s">
+      <c r="C152" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="D150" s="6" t="s">
+      <c r="D152" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E150" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F150" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G150" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="10" t="s">
+      <c r="E152" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G152" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="B153" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C151" s="8" t="s">
+      <c r="C153" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D151" s="6"/>
-      <c r="E151" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G151" s="4" t="s">
+      <c r="D153" s="6"/>
+      <c r="E153" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F153" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G153" s="4" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G151" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G153" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>